<commit_message>
Changed to good data
</commit_message>
<xml_diff>
--- a/sample mounting.xlsx
+++ b/sample mounting.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="86">
   <si>
     <t xml:space="preserve">Sample Mixture</t>
   </si>
@@ -252,26 +252,41 @@
     <t xml:space="preserve">Fractured</t>
   </si>
   <si>
+    <t xml:space="preserve">Permeable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vol in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume de Al2O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume dans final</t>
+  </si>
+  <si>
     <t xml:space="preserve">Porosité
 Ouverte</t>
   </si>
   <si>
-    <t xml:space="preserve">Sans Isostatic (50Mpa)</t>
+    <t xml:space="preserve">travailler qu’avec ça</t>
   </si>
   <si>
-    <t xml:space="preserve">PMMA (µm)</t>
+    <t xml:space="preserve">Avec Iso (150MPa + Isostatic 3500 bar press)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
   </si>
   <si>
     <t xml:space="preserve">Impermeable</t>
   </si>
   <si>
-    <t xml:space="preserve">Avec Iso (150MPa + Isostatic 3500 bar press)</t>
-  </si>
-  <si>
     <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permeable</t>
   </si>
   <si>
     <t xml:space="preserve">100-200 (75%) 200-400(25%)</t>
@@ -309,7 +324,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -404,6 +419,36 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFE0C2CD"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFE0C2CD"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFE0C2CD"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FFE0C2CD"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -447,7 +492,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,13 +538,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
-        <bgColor rgb="FFFFE699"/>
+        <bgColor rgb="FFE0C2CD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD6DCE5"/>
         <bgColor rgb="FFDBDBDB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E905"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -511,7 +562,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFE6E905"/>
       </patternFill>
     </fill>
   </fills>
@@ -675,7 +726,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="262">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1408,39 +1459,319 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="6" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="7" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1469,7 +1800,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFA9D18E"/>
+      <rgbColor rgb="FFE0C2CD"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1481,7 +1812,7 @@
       <rgbColor rgb="FFBDD7EE"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFE6E905"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -1491,7 +1822,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFD6DCE5"/>
       <rgbColor rgb="FFFFE699"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFA9D18E"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF8CBAD"/>
@@ -1527,13 +1858,13 @@
       <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="95"/>
   </cols>
@@ -4460,10 +4791,10 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.14"/>
@@ -5719,7 +6050,7 @@
       <c r="O29" s="135"/>
       <c r="P29" s="91"/>
     </row>
-    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="70"/>
       <c r="B30" s="44" t="s">
         <v>55</v>
@@ -6441,67 +6772,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="E1" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="F1" s="14" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>65</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6510,55 +6822,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>45</v>
-      </c>
       <c r="D2" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>31</v>
+        <v>18.3757661480434</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0.9973</v>
+        <v>8.07766240990432</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>2.4945</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>2.6504</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>1.802</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <f aca="false">G2/((H2-I2)/F2)</f>
-        <v>2.93230180339463</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <f aca="false">((H2-G2)/(H2-I2))*100</f>
-        <v>18.3757661480434</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <f aca="false">M2-K2</f>
-        <v>8.07766240990432</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <f aca="false">(((H2-I2)-(G2/N2)*F2)/(H2-I2))*100</f>
         <v>26.4534285579477</v>
       </c>
-      <c r="N2" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <f aca="false">((G2*F2)/(N2*(H2-I2)))*100</f>
-        <v>73.5465714420523</v>
-      </c>
-      <c r="P2" s="182" t="b">
+      <c r="H2" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -6568,55 +6851,26 @@
         <v>0</v>
       </c>
       <c r="B3" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>60</v>
-      </c>
       <c r="D3" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>37.5</v>
+        <v>24.0950226244344</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0.9973</v>
+        <v>8.24888750429849</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>2.391</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>2.604</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>1.72</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <f aca="false">G3/((H3-I3)/F3)</f>
-        <v>2.69744830316742</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <f aca="false">((H3-G3)/(H3-I3))*100</f>
-        <v>24.0950226244344</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <f aca="false">M3-K3</f>
-        <v>8.24888750429849</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <f aca="false">(((H3-I3)-(G3/N3)*F3)/(H3-I3))*100</f>
         <v>32.3439101287329</v>
       </c>
-      <c r="N3" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <f aca="false">((G3*F3)/(N3*(H3-I3)))*100</f>
-        <v>67.6560898712671</v>
-      </c>
-      <c r="P3" s="182" t="b">
+      <c r="H3" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -6626,55 +6880,26 @@
         <v>0</v>
       </c>
       <c r="B4" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="D4" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>39.71</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>39.71</v>
+        <v>23.5796509468994</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.99707</v>
+        <v>9.11009689151584</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>2.1745</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>2.365</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1.5571</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <f aca="false">G4/((H4-I4)/F4)</f>
-        <v>2.68365975368239</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <f aca="false">((H4-G4)/(H4-I4))*100</f>
-        <v>23.5796509468994</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <f aca="false">M4-K4</f>
-        <v>9.11009689151584</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <f aca="false">(((H4-I4)-(G4/N4)*F4)/(H4-I4))*100</f>
         <v>32.6897478384152</v>
       </c>
-      <c r="N4" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <f aca="false">((G4*F4)/(N4*(H4-I4)))*100</f>
-        <v>67.3102521615848</v>
-      </c>
-      <c r="P4" s="182" t="b">
+      <c r="H4" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -6684,54 +6909,25 @@
         <v>0</v>
       </c>
       <c r="B5" s="0" t="n">
-        <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>70</v>
+        <v>39.71</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>39.71</v>
+        <v>27.1101921673559</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.99707</v>
+        <v>9.40859737103504</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>2.0871</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>2.31</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>1.4878</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <f aca="false">G5/((H5-I5)/F5)</f>
-        <v>2.53099586110435</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <f aca="false">((H5-G5)/(H5-I5))*100</f>
-        <v>27.1101921673559</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <f aca="false">M5-K5</f>
-        <v>9.40859737103504</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <f aca="false">(((H5-I5)-(G5/N5)*F5)/(H5-I5))*100</f>
         <v>36.5187895383909</v>
       </c>
-      <c r="N5" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <f aca="false">((G5*F5)/(N5*(H5-I5)))*100</f>
-        <v>63.4812104616091</v>
-      </c>
-      <c r="P5" s="182" t="b">
+      <c r="H5" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -6741,111 +6937,73 @@
         <v>0</v>
       </c>
       <c r="B6" s="0" t="n">
-        <f aca="false">0</f>
+        <v>60</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>25.0263496896592</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>14.0482531161043</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>39.0746028057636</v>
+      </c>
+      <c r="H6" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0.99707</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>2.0803</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>2.294</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>1.4401</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <f aca="false">G6/((H6-I6)/F6)</f>
-        <v>2.42909558613421</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <f aca="false">((H6-G6)/(H6-I6))*100</f>
-        <v>25.0263496896592</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <f aca="false">M6-K6</f>
-        <v>14.0482531161043</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <f aca="false">(((H6-I6)-(G6/N6)*F6)/(H6-I6))*100</f>
-        <v>39.0746028057636</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <f aca="false">((G6*F6)/(N6*(H6-I6)))*100</f>
-        <v>60.9253971942364</v>
-      </c>
-      <c r="P6" s="182" t="b">
-        <v>0</v>
+      <c r="L6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <f aca="false">0</f>
+        <v>40</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>39.71</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>22.0083184789067</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>13.0629407129916</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>35.0712591918983</v>
+      </c>
+      <c r="H7" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>39.71</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0.99707</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>2.1848</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>2.37</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>1.5285</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">G7/((H7-I7)/F7)</f>
-        <v>2.58870889601901</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <f aca="false">((H7-G7)/(H7-I7))*100</f>
-        <v>22.0083184789067</v>
-      </c>
       <c r="L7" s="0" t="n">
-        <f aca="false">M7-K7</f>
-        <v>13.0629407129916</v>
+        <v>0.7</v>
       </c>
       <c r="M7" s="0" t="n">
-        <f aca="false">(((H7-I7)-(G7/N7)*F7)/(H7-I7))*100</f>
-        <v>35.0712591918983</v>
+        <f aca="false">1+L7</f>
+        <v>1.7</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O7" s="0" t="n">
-        <f aca="false">((G7*F7)/(N7*(H7-I7)))*100</f>
-        <v>64.9287408081017</v>
-      </c>
-      <c r="P7" s="182" t="b">
-        <v>0</v>
+        <f aca="false">L7/M7</f>
+        <v>0.411764705882353</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6854,113 +7012,56 @@
         <v>0</v>
       </c>
       <c r="B8" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="D8" s="0" t="n">
+        <f aca="false">60</f>
         <v>60</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="E8" s="0" t="n">
+        <v>45.9918616480163</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>5.36086844809213</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>51.3527300961084</v>
+      </c>
+      <c r="H8" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>1.9103</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>2.3624</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>1.3794</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <f aca="false">G8/((H8-I8)/F8)</f>
-        <v>1.93956665106816</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <f aca="false">((H8-G8)/(H8-I8))*100</f>
-        <v>45.9918616480163</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <f aca="false">M8-K8</f>
-        <v>5.36086844809213</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <f aca="false">(((H8-I8)-(G8/N8)*F8)/(H8-I8))*100</f>
-        <v>51.3527300961084</v>
-      </c>
-      <c r="N8" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O8" s="0" t="n">
-        <f aca="false">((G8*F8)/(N8*(H8-I8)))*100</f>
-        <v>48.6472699038916</v>
-      </c>
-      <c r="P8" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>30</v>
-      </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">60</f>
+        <v>60</v>
       </c>
       <c r="E9" s="0" t="n">
-        <f aca="false">0.6</f>
-        <v>0.6</v>
+        <v>43.820110136651</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.99806</v>
+        <v>5.77465253814649</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>1.9745</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>2.4042</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>1.4236</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <f aca="false">G9/((H9-I9)/F9)</f>
-        <v>2.00965681215582</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <f aca="false">((H9-G9)/(H9-I9))*100</f>
-        <v>43.820110136651</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <f aca="false">M9-K9</f>
-        <v>5.77465253814649</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <f aca="false">(((H9-I9)-(G9/N9)*F9)/(H9-I9))*100</f>
         <v>49.5947626747975</v>
       </c>
-      <c r="N9" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <f aca="false">((G9*F9)/(N9*(H9-I9)))*100</f>
-        <v>50.4052373252025</v>
-      </c>
-      <c r="P9" s="182" t="b">
+      <c r="H9" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -6970,250 +7071,121 @@
         <v>0</v>
       </c>
       <c r="B10" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="D10" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="H10" s="182" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="P10" s="182" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="D11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>11.5911485774499</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>30.4399320446879</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>42.0310806221378</v>
+      </c>
+      <c r="H11" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C12" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="0" t="n">
+      <c r="D12" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>2.1977</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>2.3077</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>1.3587</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <f aca="false">G11/((H11-I11)/F11)</f>
-        <v>2.31122081559536</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <f aca="false">((H11-G11)/(H11-I11))*100</f>
-        <v>11.5911485774499</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <f aca="false">M11-K11</f>
-        <v>30.4399320446879</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <f aca="false">(((H11-I11)-(G11/N11)*F11)/(H11-I11))*100</f>
-        <v>42.0310806221378</v>
-      </c>
-      <c r="N11" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <f aca="false">((G11*F11)/(N11*(H11-I11)))*100</f>
-        <v>57.9689193778622</v>
-      </c>
-      <c r="P11" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
       <c r="E12" s="0" t="n">
-        <v>50</v>
+        <v>10.4033970276009</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.99802</v>
+        <v>30.4980443341071</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>2.3352</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>2.4381</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>1.449</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <f aca="false">G12/((H12-I12)/F12)</f>
-        <v>2.35625953290871</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <f aca="false">((H12-G12)/(H12-I12))*100</f>
-        <v>10.4033970276009</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <f aca="false">M12-K12</f>
-        <v>30.4980443341071</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <f aca="false">(((H12-I12)-(G12/N12)*F12)/(H12-I12))*100</f>
         <v>40.9014413617079</v>
       </c>
-      <c r="N12" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <f aca="false">((G12*F12)/(N12*(H12-I12)))*100</f>
-        <v>59.0985586382921</v>
-      </c>
-      <c r="P12" s="182" t="b">
+      <c r="H12" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>60</v>
+        <v>32.5</v>
       </c>
       <c r="B13" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="D13" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="H13" s="182" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="B14" s="0" t="n">
         <v>60</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>2.0576</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>2.4361</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>1.3862</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <f aca="false">G13/((H13-I13)/F13)</f>
-        <v>1.95592528050291</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <f aca="false">((H13-G13)/(H13-I13))*100</f>
-        <v>36.0510524811887</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <f aca="false">M13-K13</f>
-        <v>14.8913784066241</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <f aca="false">(((H13-I13)-(G13/N13)*F13)/(H13-I13))*100</f>
-        <v>50.9424308878128</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <f aca="false">((G13*F13)/(N13*(H13-I13)))*100</f>
-        <v>49.0575691121872</v>
-      </c>
-      <c r="P13" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="D14" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>60</v>
+        <v>49.6032553407935</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.99802</v>
+        <v>3.74853808958464</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>2.021</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>2.4645</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>1.4247</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <f aca="false">G14/((H14-I14)/F14)</f>
-        <v>1.93979459511445</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <f aca="false">((H14-G14)/(H14-I14))*100</f>
-        <v>42.6524331602231</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <f aca="false">M14-K14</f>
-        <v>8.69457975388659</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <f aca="false">(((H14-I14)-(G14/N14)*F14)/(H14-I14))*100</f>
-        <v>51.3470129141097</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <f aca="false">((G14*F14)/(N14*(H14-I14)))*100</f>
-        <v>48.6529870858903</v>
-      </c>
-      <c r="P14" s="182" t="b">
+        <v>53.3517934303781</v>
+      </c>
+      <c r="H14" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -7223,1407 +7195,1045 @@
         <v>0</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>32.5</v>
+        <v>60</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="D15" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>60</v>
+      </c>
       <c r="E15" s="0" t="n">
-        <v>65</v>
-      </c>
-      <c r="P15" s="182" t="b">
-        <v>1</v>
+        <v>47.4956822107081</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>4.75292908801109</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>52.2486112987192</v>
+      </c>
+      <c r="H15" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="D16" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>70</v>
+        <v>45.4962766500051</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.99802</v>
+        <v>5.30878445839522</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>1.6498</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>2.2466</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>1.182</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <f aca="false">G16/((H16-I16)/F16)</f>
-        <v>1.54662163817396</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <f aca="false">((H16-G16)/(H16-I16))*100</f>
-        <v>56.0586135637798</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <f aca="false">M16-K16</f>
-        <v>5.1497727373498</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <f aca="false">(((H16-I16)-(G16/N16)*F16)/(H16-I16))*100</f>
-        <v>61.2083863011296</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <f aca="false">((G16*F16)/(N16*(H16-I16)))*100</f>
-        <v>38.7916136988704</v>
-      </c>
-      <c r="P16" s="182" t="b">
+        <v>50.8050611084003</v>
+      </c>
+      <c r="H16" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="D17" s="0" t="n">
-        <f aca="false">0</f>
+        <v>60</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>47.7242643315345</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>3.80309159232426</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>51.5273559238588</v>
+      </c>
+      <c r="H17" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E17" s="0" t="n">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="183"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="H21" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="184" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="184" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="184" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="184" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="184" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q23" s="185" t="s">
+        <v>48</v>
+      </c>
+      <c r="R23" s="186" t="s">
+        <v>49</v>
+      </c>
+      <c r="S23" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="T23" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="24" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G24" s="35" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H24" s="36" t="n">
+        <v>31</v>
+      </c>
+      <c r="I24" s="187" t="n">
+        <v>0.9973</v>
+      </c>
+      <c r="J24" s="188" t="n">
+        <v>2.4945</v>
+      </c>
+      <c r="K24" s="187" t="n">
+        <v>2.6504</v>
+      </c>
+      <c r="L24" s="187" t="n">
+        <v>1.802</v>
+      </c>
+      <c r="M24" s="189" t="n">
+        <f aca="false">J24/((K24-L24)/I24)</f>
+        <v>2.93230180339463</v>
+      </c>
+      <c r="N24" s="39" t="n">
+        <f aca="false">((K24-J24)/(K24-L24))*100</f>
+        <v>18.3757661480434</v>
+      </c>
+      <c r="O24" s="115" t="n">
+        <f aca="false">P24-N24</f>
+        <v>8.07766240990432</v>
+      </c>
+      <c r="P24" s="41" t="n">
+        <f aca="false">(((K24-L24)-(J24/Q24)*I24)/(K24-L24))*100</f>
+        <v>26.4534285579477</v>
+      </c>
+      <c r="Q24" s="190" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R24" s="191" t="n">
+        <f aca="false">((J24*I24)/(Q24*(K24-L24)))*100</f>
+        <v>73.5465714420523</v>
+      </c>
+      <c r="S24" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="45" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G25" s="118" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H25" s="119" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I25" s="192" t="n">
+        <v>0.9973</v>
+      </c>
+      <c r="J25" s="193" t="n">
+        <v>2.391</v>
+      </c>
+      <c r="K25" s="192" t="n">
+        <v>2.604</v>
+      </c>
+      <c r="L25" s="192" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="M25" s="194" t="n">
+        <f aca="false">J25/((K25-L25)/I25)</f>
+        <v>2.69744830316742</v>
+      </c>
+      <c r="N25" s="50" t="n">
+        <f aca="false">((K25-J25)/(K25-L25))*100</f>
+        <v>24.0950226244344</v>
+      </c>
+      <c r="O25" s="120" t="n">
+        <f aca="false">P25-N25</f>
+        <v>8.24888750429849</v>
+      </c>
+      <c r="P25" s="51" t="n">
+        <f aca="false">(((K25-L25)-(J25/Q25)*I25)/(K25-L25))*100</f>
+        <v>32.3439101287329</v>
+      </c>
+      <c r="Q25" s="195" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R25" s="196" t="n">
+        <f aca="false">((J25*I25)/(Q25*(K25-L25)))*100</f>
+        <v>67.6560898712671</v>
+      </c>
+      <c r="S25" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="27" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G26" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H26" s="62" t="n">
+        <v>39.71</v>
+      </c>
+      <c r="I26" s="197" t="n">
+        <v>0.99707</v>
+      </c>
+      <c r="J26" s="198" t="n">
+        <v>2.1745</v>
+      </c>
+      <c r="K26" s="197" t="n">
+        <v>2.365</v>
+      </c>
+      <c r="L26" s="197" t="n">
+        <v>1.5571</v>
+      </c>
+      <c r="M26" s="199" t="n">
+        <f aca="false">J26/((K26-L26)/I26)</f>
+        <v>2.68365975368239</v>
+      </c>
+      <c r="N26" s="65" t="n">
+        <f aca="false">((K26-J26)/(K26-L26))*100</f>
+        <v>23.5796509468994</v>
+      </c>
+      <c r="O26" s="67" t="n">
+        <f aca="false">P26-N26</f>
+        <v>9.11009689151584</v>
+      </c>
+      <c r="P26" s="67" t="n">
+        <f aca="false">(((K26-L26)-(J26/Q26)*I26)/(K26-L26))*100</f>
+        <v>32.6897478384152</v>
+      </c>
+      <c r="Q26" s="200" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R26" s="201" t="n">
+        <f aca="false">((J26*I26)/(Q26*(K26-L26)))*100</f>
+        <v>67.3102521615848</v>
+      </c>
+      <c r="S26" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="76" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G27" s="77" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H27" s="107" t="n">
+        <v>39.71</v>
+      </c>
+      <c r="I27" s="202" t="n">
+        <v>0.99707</v>
+      </c>
+      <c r="J27" s="203" t="n">
+        <v>2.0871</v>
+      </c>
+      <c r="K27" s="202" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="L27" s="202" t="n">
+        <v>1.4878</v>
+      </c>
+      <c r="M27" s="204" t="n">
+        <f aca="false">J27/((K27-L27)/I27)</f>
+        <v>2.53099586110435</v>
+      </c>
+      <c r="N27" s="81" t="n">
+        <f aca="false">((K27-J27)/(K27-L27))*100</f>
+        <v>27.1101921673559</v>
+      </c>
+      <c r="O27" s="83" t="n">
+        <f aca="false">P27-N27</f>
+        <v>9.40859737103504</v>
+      </c>
+      <c r="P27" s="83" t="n">
+        <f aca="false">(((K27-L27)-(J27/Q27)*I27)/(K27-L27))*100</f>
+        <v>36.5187895383909</v>
+      </c>
+      <c r="Q27" s="205" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R27" s="206" t="n">
+        <f aca="false">((J27*I27)/(Q27*(K27-L27)))*100</f>
+        <v>63.4812104616091</v>
+      </c>
+      <c r="S27" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="27" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G28" s="94" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H28" s="95" t="n">
+        <v>43</v>
+      </c>
+      <c r="I28" s="207" t="n">
+        <v>0.99707</v>
+      </c>
+      <c r="J28" s="208" t="n">
+        <v>2.0803</v>
+      </c>
+      <c r="K28" s="209" t="n">
+        <v>2.294</v>
+      </c>
+      <c r="L28" s="210" t="n">
+        <v>1.4401</v>
+      </c>
+      <c r="M28" s="211" t="n">
+        <f aca="false">J28/((K28-L28)/I28)</f>
+        <v>2.42909558613421</v>
+      </c>
+      <c r="N28" s="125" t="n">
+        <f aca="false">((K28-J28)/(K28-L28))*100</f>
+        <v>25.0263496896592</v>
+      </c>
+      <c r="O28" s="126" t="n">
+        <f aca="false">P28-N28</f>
+        <v>14.0482531161043</v>
+      </c>
+      <c r="P28" s="69" t="n">
+        <f aca="false">(((K28-L28)-(J28/Q28)*I28)/(K28-L28))*100</f>
+        <v>39.0746028057636</v>
+      </c>
+      <c r="Q28" s="212" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R28" s="213" t="n">
+        <f aca="false">((J28*I28)/(Q28*(K28-L28)))*100</f>
+        <v>60.9253971942364</v>
+      </c>
+      <c r="S28" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="27" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G29" s="127"/>
+      <c r="I29" s="214"/>
+      <c r="J29" s="215"/>
+      <c r="K29" s="216"/>
+      <c r="L29" s="217"/>
+      <c r="M29" s="218"/>
+      <c r="N29" s="133"/>
+      <c r="O29" s="134"/>
+      <c r="P29" s="91"/>
+      <c r="Q29" s="219"/>
+      <c r="R29" s="220"/>
+      <c r="S29" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="45" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G30" s="46" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H30" s="47" t="n">
+        <v>39.71</v>
+      </c>
+      <c r="I30" s="221" t="n">
+        <v>0.99707</v>
+      </c>
+      <c r="J30" s="222" t="n">
+        <v>2.1848</v>
+      </c>
+      <c r="K30" s="222" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="L30" s="222" t="n">
+        <v>1.5285</v>
+      </c>
+      <c r="M30" s="223" t="n">
+        <f aca="false">J30/((K30-L30)/I30)</f>
+        <v>2.58870889601901</v>
+      </c>
+      <c r="N30" s="139" t="n">
+        <f aca="false">((K30-J30)/(K30-L30))*100</f>
+        <v>22.0083184789067</v>
+      </c>
+      <c r="O30" s="55" t="n">
+        <f aca="false">P30-N30</f>
+        <v>13.0629407129916</v>
+      </c>
+      <c r="P30" s="140" t="n">
+        <f aca="false">(((K30-L30)-(J30/Q30)*I30)/(K30-L30))*100</f>
+        <v>35.0712591918983</v>
+      </c>
+      <c r="Q30" s="224" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R30" s="225" t="n">
+        <f aca="false">((J30*I30)/(Q30*(K30-L30)))*100</f>
+        <v>64.9287408081017</v>
+      </c>
+      <c r="S30" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="45" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G31" s="141"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="226"/>
+      <c r="J31" s="227"/>
+      <c r="K31" s="227"/>
+      <c r="L31" s="227"/>
+      <c r="M31" s="228"/>
+      <c r="N31" s="146"/>
+      <c r="O31" s="147"/>
+      <c r="P31" s="148"/>
+      <c r="Q31" s="229"/>
+      <c r="R31" s="230"/>
+      <c r="S31" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="137" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="150" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G32" s="151"/>
+      <c r="H32" s="152"/>
+      <c r="I32" s="226"/>
+      <c r="J32" s="227"/>
+      <c r="K32" s="227"/>
+      <c r="L32" s="227"/>
+      <c r="M32" s="228"/>
+      <c r="N32" s="146"/>
+      <c r="O32" s="147"/>
+      <c r="P32" s="148"/>
+      <c r="Q32" s="229"/>
+      <c r="R32" s="230"/>
+      <c r="S32" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="121" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="153"/>
+      <c r="G33" s="153"/>
+      <c r="H33" s="154" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I33" s="197" t="n">
+        <v>0.99806</v>
+      </c>
+      <c r="J33" s="198" t="n">
+        <v>1.9103</v>
+      </c>
+      <c r="K33" s="197" t="n">
+        <v>2.3624</v>
+      </c>
+      <c r="L33" s="197" t="n">
+        <v>1.3794</v>
+      </c>
+      <c r="M33" s="199" t="n">
+        <f aca="false">J33/((K33-L33)/I33)</f>
+        <v>1.93956665106816</v>
+      </c>
+      <c r="N33" s="65" t="n">
+        <f aca="false">((K33-J33)/(K33-L33))*100</f>
+        <v>45.9918616480163</v>
+      </c>
+      <c r="O33" s="66" t="n">
+        <f aca="false">P33-N33</f>
+        <v>5.36086844809213</v>
+      </c>
+      <c r="P33" s="67" t="n">
+        <f aca="false">(((K33-L33)-(J33/Q33)*I33)/(K33-L33))*100</f>
+        <v>51.3527300961084</v>
+      </c>
+      <c r="Q33" s="212" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R33" s="213" t="n">
+        <f aca="false">((J33*I33)/(Q33*(K33-L33)))*100</f>
+        <v>48.6472699038916</v>
+      </c>
+      <c r="S33" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="155" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
+      <c r="H34" s="154"/>
+      <c r="I34" s="197" t="n">
+        <v>0.99806</v>
+      </c>
+      <c r="J34" s="197" t="n">
+        <v>1.9745</v>
+      </c>
+      <c r="K34" s="197" t="n">
+        <v>2.4042</v>
+      </c>
+      <c r="L34" s="231" t="n">
+        <v>1.4236</v>
+      </c>
+      <c r="M34" s="199" t="n">
+        <f aca="false">J34/((K34-L34)/I34)</f>
+        <v>2.00965681215582</v>
+      </c>
+      <c r="N34" s="65" t="n">
+        <f aca="false">((K34-J34)/(K34-L34))*100</f>
+        <v>43.820110136651</v>
+      </c>
+      <c r="O34" s="72" t="n">
+        <f aca="false">P34-N34</f>
+        <v>5.77465253814649</v>
+      </c>
+      <c r="P34" s="67" t="n">
+        <f aca="false">(((K34-L34)-(J34/Q34)*I34)/(K34-L34))*100</f>
+        <v>49.5947626747975</v>
+      </c>
+      <c r="Q34" s="200" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R34" s="201" t="n">
+        <f aca="false">((J34*I34)/(Q34*(K34-L34)))*100</f>
+        <v>50.4052373252025</v>
+      </c>
+      <c r="S34" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="153"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="62" t="n">
+        <v>70</v>
+      </c>
+      <c r="I35" s="232"/>
+      <c r="J35" s="232"/>
+      <c r="K35" s="232"/>
+      <c r="L35" s="232"/>
+      <c r="M35" s="232"/>
+      <c r="N35" s="153"/>
+      <c r="O35" s="153"/>
+      <c r="P35" s="153"/>
+      <c r="Q35" s="232"/>
+      <c r="R35" s="232"/>
+      <c r="S35" s="182" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E36" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" s="153"/>
+      <c r="G36" s="153"/>
+      <c r="H36" s="62" t="n">
+        <v>50</v>
+      </c>
+      <c r="I36" s="233" t="n">
         <v>0.99802</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>1.4072</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>1.9133</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>1.0109</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <f aca="false">G17/((H17-I17)/F17)</f>
-        <v>1.55630955673759</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <f aca="false">((H17-G17)/(H17-I17))*100</f>
-        <v>56.0837765957447</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <f aca="false">M17-K17</f>
-        <v>4.88162203135369</v>
-      </c>
-      <c r="M17" s="0" t="n">
-        <f aca="false">(((H17-I17)-(G17/N17)*F17)/(H17-I17))*100</f>
-        <v>60.9653986270984</v>
-      </c>
-      <c r="N17" s="0" t="n">
+      <c r="J36" s="233" t="n">
+        <v>2.1977</v>
+      </c>
+      <c r="K36" s="234" t="n">
+        <v>2.3077</v>
+      </c>
+      <c r="L36" s="234" t="n">
+        <v>1.3587</v>
+      </c>
+      <c r="M36" s="235" t="n">
+        <f aca="false">J36/((K36-L36)/I36)</f>
+        <v>2.31122081559536</v>
+      </c>
+      <c r="N36" s="119" t="n">
+        <f aca="false">((K36-J36)/(K36-L36))*100</f>
+        <v>11.5911485774499</v>
+      </c>
+      <c r="O36" s="159" t="n">
+        <f aca="false">P36-N36</f>
+        <v>30.4399320446879</v>
+      </c>
+      <c r="P36" s="160" t="n">
+        <f aca="false">(((K36-L36)-(J36/Q36)*I36)/(K36-L36))*100</f>
+        <v>42.0310806221378</v>
+      </c>
+      <c r="Q36" s="236" t="n">
         <v>3.987</v>
       </c>
-      <c r="O17" s="0" t="n">
-        <f aca="false">((G17*F17)/(N17*(H17-I17)))*100</f>
-        <v>39.0346013729016</v>
-      </c>
-      <c r="P17" s="182" t="b">
+      <c r="R36" s="237" t="n">
+        <f aca="false">((J36*I36)/(Q36*(K36-L36)))*100</f>
+        <v>57.9689193778622</v>
+      </c>
+      <c r="S36" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>1.8318</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>2.3194</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>1.3364</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <f aca="false">G18/((H18-I18)/F18)</f>
-        <v>1.85986399593082</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <f aca="false">((H18-G18)/(H18-I18))*100</f>
-        <v>49.6032553407935</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <f aca="false">M18-K18</f>
-        <v>3.74853808958464</v>
-      </c>
-      <c r="M18" s="0" t="n">
-        <f aca="false">(((H18-I18)-(G18/N18)*F18)/(H18-I18))*100</f>
-        <v>53.3517934303781</v>
-      </c>
-      <c r="N18" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O18" s="0" t="n">
-        <f aca="false">((G18*F18)/(N18*(H18-I18)))*100</f>
-        <v>46.6482065696219</v>
-      </c>
-      <c r="P18" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>1.8776</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>2.3451</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>1.3608</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <f aca="false">G19/((H19-I19)/F19)</f>
-        <v>1.90384786752007</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <f aca="false">((H19-G19)/(H19-I19))*100</f>
-        <v>47.4956822107081</v>
-      </c>
-      <c r="L19" s="0" t="n">
-        <f aca="false">M19-K19</f>
-        <v>4.75292908801109</v>
-      </c>
-      <c r="M19" s="0" t="n">
-        <f aca="false">(((H19-I19)-(G19/N19)*F19)/(H19-I19))*100</f>
-        <v>52.2486112987192</v>
-      </c>
-      <c r="N19" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O19" s="0" t="n">
-        <f aca="false">((G19*F19)/(N19*(H19-I19)))*100</f>
-        <v>47.7513887012808</v>
-      </c>
-      <c r="P19" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>1.9265</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>2.3725</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>1.3922</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <f aca="false">G20/((H20-I20)/F20)</f>
-        <v>1.96140221360808</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <f aca="false">((H20-G20)/(H20-I20))*100</f>
-        <v>45.4962766500051</v>
-      </c>
-      <c r="L20" s="0" t="n">
-        <f aca="false">M20-K20</f>
-        <v>5.30878445839522</v>
-      </c>
-      <c r="M20" s="0" t="n">
-        <f aca="false">(((H20-I20)-(G20/N20)*F20)/(H20-I20))*100</f>
-        <v>50.8050611084003</v>
-      </c>
-      <c r="N20" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O20" s="0" t="n">
-        <f aca="false">((G20*F20)/(N20*(H20-I20)))*100</f>
-        <v>49.1949388915997</v>
-      </c>
-      <c r="P20" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>1.9017</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>2.3704</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>1.3883</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <f aca="false">G21/((H21-I21)/F21)</f>
-        <v>1.93260431931575</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <f aca="false">((H21-G21)/(H21-I21))*100</f>
-        <v>47.7242643315345</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <f aca="false">M21-K21</f>
-        <v>3.80309159232426</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <f aca="false">(((H21-I21)-(G21/N21)*F21)/(H21-I21))*100</f>
-        <v>51.5273559238588</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="O21" s="0" t="n">
-        <f aca="false">((G21*F21)/(N21*(H21-I21)))*100</f>
-        <v>48.4726440761413</v>
-      </c>
-      <c r="P21" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M27" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="N27" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="O27" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="P27" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q27" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="R27" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="S27" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="113" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="24" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="G28" s="35" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="H28" s="36" t="n">
-        <v>31</v>
-      </c>
-      <c r="I28" s="22" t="n">
-        <v>0.9973</v>
-      </c>
-      <c r="J28" s="37" t="n">
-        <v>2.4945</v>
-      </c>
-      <c r="K28" s="22" t="n">
-        <v>2.6504</v>
-      </c>
-      <c r="L28" s="22" t="n">
-        <v>1.802</v>
-      </c>
-      <c r="M28" s="38" t="n">
-        <f aca="false">J28/((K28-L28)/I28)</f>
-        <v>2.93230180339463</v>
-      </c>
-      <c r="N28" s="39" t="n">
-        <f aca="false">((K28-J28)/(K28-L28))*100</f>
-        <v>18.3757661480434</v>
-      </c>
-      <c r="O28" s="115" t="n">
-        <f aca="false">P28-N28</f>
-        <v>8.07766240990432</v>
-      </c>
-      <c r="P28" s="41" t="n">
-        <f aca="false">(((K28-L28)-(J28/Q28)*I28)/(K28-L28))*100</f>
-        <v>26.4534285579477</v>
-      </c>
-      <c r="Q28" s="116" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R28" s="117" t="n">
-        <f aca="false">((J28*I28)/(Q28*(K28-L28)))*100</f>
-        <v>73.5465714420523</v>
-      </c>
-      <c r="S28" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="45" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="G29" s="118" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H29" s="119" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="I29" s="44" t="n">
-        <v>0.9973</v>
-      </c>
-      <c r="J29" s="48" t="n">
-        <v>2.391</v>
-      </c>
-      <c r="K29" s="44" t="n">
-        <v>2.604</v>
-      </c>
-      <c r="L29" s="44" t="n">
-        <v>1.72</v>
-      </c>
-      <c r="M29" s="49" t="n">
-        <f aca="false">J29/((K29-L29)/I29)</f>
-        <v>2.69744830316742</v>
-      </c>
-      <c r="N29" s="50" t="n">
-        <f aca="false">((K29-J29)/(K29-L29))*100</f>
-        <v>24.0950226244344</v>
-      </c>
-      <c r="O29" s="120" t="n">
-        <f aca="false">P29-N29</f>
-        <v>8.24888750429849</v>
-      </c>
-      <c r="P29" s="51" t="n">
-        <f aca="false">(((K29-L29)-(J29/Q29)*I29)/(K29-L29))*100</f>
-        <v>32.3439101287329</v>
-      </c>
-      <c r="Q29" s="52" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R29" s="51" t="n">
-        <f aca="false">((J29*I29)/(Q29*(K29-L29)))*100</f>
-        <v>67.6560898712671</v>
-      </c>
-      <c r="S29" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="27" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G30" s="59" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="H30" s="62" t="n">
-        <v>39.71</v>
-      </c>
-      <c r="I30" s="60" t="n">
-        <v>0.99707</v>
-      </c>
-      <c r="J30" s="63" t="n">
-        <v>2.1745</v>
-      </c>
-      <c r="K30" s="60" t="n">
-        <v>2.365</v>
-      </c>
-      <c r="L30" s="60" t="n">
-        <v>1.5571</v>
-      </c>
-      <c r="M30" s="64" t="n">
-        <f aca="false">J30/((K30-L30)/I30)</f>
-        <v>2.68365975368239</v>
-      </c>
-      <c r="N30" s="65" t="n">
-        <f aca="false">((K30-J30)/(K30-L30))*100</f>
-        <v>23.5796509468994</v>
-      </c>
-      <c r="O30" s="67" t="n">
-        <f aca="false">P30-N30</f>
-        <v>9.11009689151584</v>
-      </c>
-      <c r="P30" s="67" t="n">
-        <f aca="false">(((K30-L30)-(J30/Q30)*I30)/(K30-L30))*100</f>
-        <v>32.6897478384152</v>
-      </c>
-      <c r="Q30" s="73" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R30" s="67" t="n">
-        <f aca="false">((J30*I30)/(Q30*(K30-L30)))*100</f>
-        <v>67.3102521615848</v>
-      </c>
-      <c r="S30" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="76" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G31" s="77" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="H31" s="107" t="n">
-        <v>39.71</v>
-      </c>
-      <c r="I31" s="75" t="n">
-        <v>0.99707</v>
-      </c>
-      <c r="J31" s="79" t="n">
-        <v>2.0871</v>
-      </c>
-      <c r="K31" s="75" t="n">
-        <v>2.31</v>
-      </c>
-      <c r="L31" s="75" t="n">
-        <v>1.4878</v>
-      </c>
-      <c r="M31" s="80" t="n">
-        <f aca="false">J31/((K31-L31)/I31)</f>
-        <v>2.53099586110435</v>
-      </c>
-      <c r="N31" s="81" t="n">
-        <f aca="false">((K31-J31)/(K31-L31))*100</f>
-        <v>27.1101921673559</v>
-      </c>
-      <c r="O31" s="83" t="n">
-        <f aca="false">P31-N31</f>
-        <v>9.40859737103504</v>
-      </c>
-      <c r="P31" s="83" t="n">
-        <f aca="false">(((K31-L31)-(J31/Q31)*I31)/(K31-L31))*100</f>
-        <v>36.5187895383909</v>
-      </c>
-      <c r="Q31" s="84" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R31" s="83" t="n">
-        <f aca="false">((J31*I31)/(Q31*(K31-L31)))*100</f>
-        <v>63.4812104616091</v>
-      </c>
-      <c r="S31" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="27" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="G32" s="94" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="H32" s="95" t="n">
-        <v>43</v>
-      </c>
-      <c r="I32" s="121" t="n">
-        <v>0.99707</v>
-      </c>
-      <c r="J32" s="122" t="n">
-        <v>2.0803</v>
-      </c>
-      <c r="K32" s="123" t="n">
-        <v>2.294</v>
-      </c>
-      <c r="L32" s="85" t="n">
-        <v>1.4401</v>
-      </c>
-      <c r="M32" s="124" t="n">
-        <f aca="false">J32/((K32-L32)/I32)</f>
-        <v>2.42909558613421</v>
-      </c>
-      <c r="N32" s="125" t="n">
-        <f aca="false">((K32-J32)/(K32-L32))*100</f>
-        <v>25.0263496896592</v>
-      </c>
-      <c r="O32" s="126" t="n">
-        <f aca="false">P32-N32</f>
-        <v>14.0482531161043</v>
-      </c>
-      <c r="P32" s="69" t="n">
-        <f aca="false">(((K32-L32)-(J32/Q32)*I32)/(K32-L32))*100</f>
-        <v>39.0746028057636</v>
-      </c>
-      <c r="Q32" s="68" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R32" s="69" t="n">
-        <f aca="false">((J32*I32)/(Q32*(K32-L32)))*100</f>
-        <v>60.9253971942364</v>
-      </c>
-      <c r="S32" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="60" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="27" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G33" s="127"/>
-      <c r="H33" s="128"/>
-      <c r="I33" s="129"/>
-      <c r="J33" s="130"/>
-      <c r="K33" s="131"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="132"/>
-      <c r="N33" s="133"/>
-      <c r="O33" s="134"/>
-      <c r="P33" s="91"/>
-      <c r="Q33" s="135"/>
-      <c r="R33" s="91"/>
-      <c r="S33" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="45" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G34" s="46" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="H34" s="47" t="n">
-        <v>39.71</v>
-      </c>
-      <c r="I34" s="136" t="n">
-        <v>0.99707</v>
-      </c>
-      <c r="J34" s="137" t="n">
-        <v>2.1848</v>
-      </c>
-      <c r="K34" s="137" t="n">
-        <v>2.37</v>
-      </c>
-      <c r="L34" s="137" t="n">
-        <v>1.5285</v>
-      </c>
-      <c r="M34" s="138" t="n">
-        <f aca="false">J34/((K34-L34)/I34)</f>
-        <v>2.58870889601901</v>
-      </c>
-      <c r="N34" s="139" t="n">
-        <f aca="false">((K34-J34)/(K34-L34))*100</f>
-        <v>22.0083184789067</v>
-      </c>
-      <c r="O34" s="55" t="n">
-        <f aca="false">P34-N34</f>
-        <v>13.0629407129916</v>
-      </c>
-      <c r="P34" s="140" t="n">
-        <f aca="false">(((K34-L34)-(J34/Q34)*I34)/(K34-L34))*100</f>
-        <v>35.0712591918983</v>
-      </c>
-      <c r="Q34" s="56" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R34" s="55" t="n">
-        <f aca="false">((J34*I34)/(Q34*(K34-L34)))*100</f>
-        <v>64.9287408081017</v>
-      </c>
-      <c r="S34" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="45" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G35" s="141"/>
-      <c r="H35" s="142"/>
-      <c r="I35" s="143"/>
-      <c r="J35" s="144"/>
-      <c r="K35" s="144"/>
-      <c r="L35" s="144"/>
-      <c r="M35" s="145"/>
-      <c r="N35" s="146"/>
-      <c r="O35" s="147"/>
-      <c r="P35" s="148"/>
-      <c r="Q35" s="149"/>
-      <c r="R35" s="147"/>
-      <c r="S35" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="137" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="150" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G36" s="151"/>
-      <c r="H36" s="152"/>
-      <c r="I36" s="143"/>
-      <c r="J36" s="144"/>
-      <c r="K36" s="144"/>
-      <c r="L36" s="144"/>
-      <c r="M36" s="145"/>
-      <c r="N36" s="146"/>
-      <c r="O36" s="147"/>
-      <c r="P36" s="148"/>
-      <c r="Q36" s="149"/>
-      <c r="R36" s="147"/>
-      <c r="S36" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="121" t="s">
-        <v>57</v>
-      </c>
+      <c r="E37" s="71"/>
       <c r="F37" s="153"/>
       <c r="G37" s="153"/>
-      <c r="H37" s="154" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I37" s="60" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="J37" s="63" t="n">
-        <v>1.9103</v>
-      </c>
-      <c r="K37" s="60" t="n">
-        <v>2.3624</v>
-      </c>
-      <c r="L37" s="60" t="n">
-        <v>1.3794</v>
-      </c>
-      <c r="M37" s="64" t="n">
+      <c r="H37" s="62"/>
+      <c r="I37" s="233" t="n">
+        <v>0.99802</v>
+      </c>
+      <c r="J37" s="238" t="n">
+        <v>2.3352</v>
+      </c>
+      <c r="K37" s="234" t="n">
+        <v>2.4381</v>
+      </c>
+      <c r="L37" s="234" t="n">
+        <v>1.449</v>
+      </c>
+      <c r="M37" s="235" t="n">
         <f aca="false">J37/((K37-L37)/I37)</f>
-        <v>1.93956665106816</v>
-      </c>
-      <c r="N37" s="65" t="n">
+        <v>2.35625953290871</v>
+      </c>
+      <c r="N37" s="119" t="n">
         <f aca="false">((K37-J37)/(K37-L37))*100</f>
-        <v>45.9918616480163</v>
-      </c>
-      <c r="O37" s="66" t="n">
+        <v>10.4033970276009</v>
+      </c>
+      <c r="O37" s="159" t="n">
         <f aca="false">P37-N37</f>
-        <v>5.36086844809213</v>
-      </c>
-      <c r="P37" s="67" t="n">
+        <v>30.4980443341071</v>
+      </c>
+      <c r="P37" s="160" t="n">
         <f aca="false">(((K37-L37)-(J37/Q37)*I37)/(K37-L37))*100</f>
-        <v>51.3527300961084</v>
-      </c>
-      <c r="Q37" s="68" t="n">
+        <v>40.9014413617079</v>
+      </c>
+      <c r="Q37" s="236" t="n">
         <v>3.987</v>
       </c>
-      <c r="R37" s="69" t="n">
+      <c r="R37" s="237" t="n">
         <f aca="false">((J37*I37)/(Q37*(K37-L37)))*100</f>
-        <v>48.6472699038916</v>
-      </c>
-      <c r="S37" s="182" t="b">
+        <v>59.0985586382921</v>
+      </c>
+      <c r="S37" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="155" t="s">
-        <v>63</v>
-      </c>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="60"/>
       <c r="F38" s="153"/>
       <c r="G38" s="153"/>
-      <c r="H38" s="154"/>
-      <c r="I38" s="60" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="J38" s="60" t="n">
-        <v>1.9745</v>
-      </c>
-      <c r="K38" s="60" t="n">
-        <v>2.4042</v>
-      </c>
-      <c r="L38" s="71" t="n">
-        <v>1.4236</v>
-      </c>
-      <c r="M38" s="64" t="n">
-        <f aca="false">J38/((K38-L38)/I38)</f>
-        <v>2.00965681215582</v>
-      </c>
-      <c r="N38" s="65" t="n">
-        <f aca="false">((K38-J38)/(K38-L38))*100</f>
-        <v>43.820110136651</v>
-      </c>
-      <c r="O38" s="72" t="n">
-        <f aca="false">P38-N38</f>
-        <v>5.77465253814649</v>
-      </c>
-      <c r="P38" s="67" t="n">
-        <f aca="false">(((K38-L38)-(J38/Q38)*I38)/(K38-L38))*100</f>
-        <v>49.5947626747975</v>
-      </c>
-      <c r="Q38" s="73" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R38" s="67" t="n">
-        <f aca="false">((J38*I38)/(Q38*(K38-L38)))*100</f>
-        <v>50.4052373252025</v>
-      </c>
-      <c r="S38" s="182" t="b">
-        <v>0</v>
-      </c>
+      <c r="H38" s="62"/>
+      <c r="I38" s="239"/>
+      <c r="J38" s="239"/>
+      <c r="K38" s="239"/>
+      <c r="L38" s="239"/>
+      <c r="M38" s="240"/>
+      <c r="N38" s="165"/>
+      <c r="O38" s="166"/>
+      <c r="P38" s="167"/>
+      <c r="Q38" s="241"/>
+      <c r="R38" s="242"/>
+      <c r="S38" s="182"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="60" t="s">
-        <v>57</v>
-      </c>
+      <c r="E39" s="60"/>
       <c r="F39" s="153"/>
       <c r="G39" s="153"/>
-      <c r="H39" s="62" t="n">
-        <v>70</v>
-      </c>
-      <c r="I39" s="153"/>
-      <c r="J39" s="153"/>
-      <c r="K39" s="153"/>
-      <c r="L39" s="153"/>
-      <c r="M39" s="153"/>
-      <c r="N39" s="153"/>
-      <c r="O39" s="153"/>
-      <c r="P39" s="153"/>
-      <c r="Q39" s="153"/>
-      <c r="R39" s="153"/>
-      <c r="S39" s="182" t="b">
-        <v>1</v>
-      </c>
+      <c r="H39" s="62"/>
+      <c r="I39" s="239"/>
+      <c r="J39" s="243"/>
+      <c r="K39" s="244"/>
+      <c r="L39" s="244"/>
+      <c r="M39" s="240"/>
+      <c r="N39" s="165"/>
+      <c r="O39" s="166"/>
+      <c r="P39" s="167"/>
+      <c r="Q39" s="241"/>
+      <c r="R39" s="242"/>
+      <c r="S39" s="182"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E40" s="71" t="s">
+      <c r="E40" s="171" t="s">
         <v>63</v>
       </c>
       <c r="F40" s="153"/>
       <c r="G40" s="153"/>
-      <c r="H40" s="62" t="n">
-        <v>50</v>
-      </c>
-      <c r="I40" s="156" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="J40" s="156" t="n">
-        <v>2.1977</v>
-      </c>
-      <c r="K40" s="157" t="n">
-        <v>2.3077</v>
-      </c>
-      <c r="L40" s="157" t="n">
-        <v>1.3587</v>
-      </c>
-      <c r="M40" s="158" t="n">
-        <f aca="false">J40/((K40-L40)/I40)</f>
-        <v>2.31122081559536</v>
-      </c>
-      <c r="N40" s="119" t="n">
-        <f aca="false">((K40-J40)/(K40-L40))*100</f>
-        <v>11.5911485774499</v>
-      </c>
-      <c r="O40" s="159" t="n">
-        <f aca="false">P40-N40</f>
-        <v>30.4399320446879</v>
-      </c>
-      <c r="P40" s="160" t="n">
-        <f aca="false">(((K40-L40)-(J40/Q40)*I40)/(K40-L40))*100</f>
-        <v>42.0310806221378</v>
-      </c>
-      <c r="Q40" s="161" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R40" s="160" t="n">
-        <f aca="false">((J40*I40)/(Q40*(K40-L40)))*100</f>
-        <v>57.9689193778622</v>
-      </c>
-      <c r="S40" s="182" t="b">
-        <v>0</v>
+      <c r="H40" s="95" t="n">
+        <v>65</v>
+      </c>
+      <c r="I40" s="231"/>
+      <c r="J40" s="245"/>
+      <c r="K40" s="246"/>
+      <c r="L40" s="246"/>
+      <c r="M40" s="247"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="175"/>
+      <c r="P40" s="176"/>
+      <c r="Q40" s="248"/>
+      <c r="R40" s="249"/>
+      <c r="S40" s="182" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="71"/>
+      <c r="E41" s="44"/>
       <c r="F41" s="153"/>
       <c r="G41" s="153"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="156" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="J41" s="162" t="n">
-        <v>2.3352</v>
-      </c>
-      <c r="K41" s="157" t="n">
-        <v>2.4381</v>
-      </c>
-      <c r="L41" s="157" t="n">
-        <v>1.449</v>
-      </c>
-      <c r="M41" s="158" t="n">
-        <f aca="false">J41/((K41-L41)/I41)</f>
-        <v>2.35625953290871</v>
-      </c>
-      <c r="N41" s="119" t="n">
-        <f aca="false">((K41-J41)/(K41-L41))*100</f>
-        <v>10.4033970276009</v>
-      </c>
-      <c r="O41" s="159" t="n">
-        <f aca="false">P41-N41</f>
-        <v>30.4980443341071</v>
-      </c>
-      <c r="P41" s="160" t="n">
-        <f aca="false">(((K41-L41)-(J41/Q41)*I41)/(K41-L41))*100</f>
-        <v>40.9014413617079</v>
-      </c>
-      <c r="Q41" s="161" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R41" s="160" t="n">
-        <f aca="false">((J41*I41)/(Q41*(K41-L41)))*100</f>
-        <v>59.0985586382921</v>
-      </c>
-      <c r="S41" s="182" t="b">
-        <v>0</v>
-      </c>
+      <c r="H41" s="178"/>
+      <c r="I41" s="233"/>
+      <c r="J41" s="234"/>
+      <c r="K41" s="234"/>
+      <c r="L41" s="234"/>
+      <c r="M41" s="235"/>
+      <c r="N41" s="119"/>
+      <c r="O41" s="159"/>
+      <c r="P41" s="160"/>
+      <c r="Q41" s="236"/>
+      <c r="R41" s="237"/>
+      <c r="S41" s="182"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E42" s="60" t="s">
-        <v>64</v>
-      </c>
+      <c r="E42" s="44"/>
       <c r="F42" s="153"/>
       <c r="G42" s="153"/>
-      <c r="H42" s="62" t="n">
-        <v>60</v>
-      </c>
-      <c r="I42" s="163" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="J42" s="163" t="n">
-        <v>2.0576</v>
-      </c>
-      <c r="K42" s="163" t="n">
-        <v>2.4361</v>
-      </c>
-      <c r="L42" s="163" t="n">
-        <v>1.3862</v>
-      </c>
-      <c r="M42" s="164" t="n">
-        <f aca="false">J42/((K42-L42)/I42)</f>
-        <v>1.95592528050291</v>
-      </c>
-      <c r="N42" s="165" t="n">
-        <f aca="false">((K42-J42)/(K42-L42))*100</f>
-        <v>36.0510524811887</v>
-      </c>
-      <c r="O42" s="166" t="n">
-        <f aca="false">P42-N42</f>
-        <v>14.8913784066241</v>
-      </c>
-      <c r="P42" s="167" t="n">
-        <f aca="false">(((K42-L42)-(J42/Q42)*I42)/(K42-L42))*100</f>
-        <v>50.9424308878128</v>
-      </c>
-      <c r="Q42" s="168" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R42" s="167" t="n">
-        <f aca="false">((J42*I42)/(Q42*(K42-L42)))*100</f>
-        <v>49.0575691121872</v>
-      </c>
-      <c r="S42" s="182" t="b">
-        <v>0</v>
-      </c>
+      <c r="H42" s="178"/>
+      <c r="I42" s="233"/>
+      <c r="J42" s="234"/>
+      <c r="K42" s="234"/>
+      <c r="L42" s="234"/>
+      <c r="M42" s="235"/>
+      <c r="N42" s="119"/>
+      <c r="O42" s="159"/>
+      <c r="P42" s="160"/>
+      <c r="Q42" s="236"/>
+      <c r="R42" s="237"/>
+      <c r="S42" s="182"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E43" s="60"/>
+      <c r="E43" s="60" t="s">
+        <v>57</v>
+      </c>
       <c r="F43" s="153"/>
       <c r="G43" s="153"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="163" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="J43" s="169" t="n">
-        <v>2.021</v>
-      </c>
-      <c r="K43" s="170" t="n">
-        <v>2.4645</v>
-      </c>
-      <c r="L43" s="170" t="n">
-        <v>1.4247</v>
-      </c>
-      <c r="M43" s="164" t="n">
+      <c r="H43" s="180" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I43" s="197" t="n">
+        <v>0.99806</v>
+      </c>
+      <c r="J43" s="231" t="n">
+        <v>1.8318</v>
+      </c>
+      <c r="K43" s="197" t="n">
+        <v>2.3194</v>
+      </c>
+      <c r="L43" s="197" t="n">
+        <v>1.3364</v>
+      </c>
+      <c r="M43" s="199" t="n">
         <f aca="false">J43/((K43-L43)/I43)</f>
-        <v>1.93979459511445</v>
-      </c>
-      <c r="N43" s="165" t="n">
+        <v>1.85986399593082</v>
+      </c>
+      <c r="N43" s="65" t="n">
         <f aca="false">((K43-J43)/(K43-L43))*100</f>
-        <v>42.6524331602231</v>
-      </c>
-      <c r="O43" s="166" t="n">
+        <v>49.6032553407935</v>
+      </c>
+      <c r="O43" s="66" t="n">
         <f aca="false">P43-N43</f>
-        <v>8.69457975388659</v>
-      </c>
-      <c r="P43" s="167" t="n">
+        <v>3.74853808958464</v>
+      </c>
+      <c r="P43" s="67" t="n">
         <f aca="false">(((K43-L43)-(J43/Q43)*I43)/(K43-L43))*100</f>
-        <v>51.3470129141097</v>
-      </c>
-      <c r="Q43" s="168" t="n">
+        <v>53.3517934303781</v>
+      </c>
+      <c r="Q43" s="212" t="n">
         <v>3.987</v>
       </c>
-      <c r="R43" s="167" t="n">
+      <c r="R43" s="213" t="n">
         <f aca="false">((J43*I43)/(Q43*(K43-L43)))*100</f>
-        <v>48.6529870858903</v>
-      </c>
-      <c r="S43" s="182" t="b">
+        <v>46.6482065696219</v>
+      </c>
+      <c r="S43" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E44" s="171" t="s">
-        <v>63</v>
-      </c>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="60"/>
       <c r="F44" s="153"/>
       <c r="G44" s="153"/>
-      <c r="H44" s="95" t="n">
-        <v>65</v>
-      </c>
-      <c r="I44" s="71"/>
-      <c r="J44" s="172"/>
-      <c r="K44" s="173"/>
-      <c r="L44" s="173"/>
-      <c r="M44" s="174"/>
-      <c r="N44" s="62"/>
-      <c r="O44" s="175"/>
-      <c r="P44" s="176"/>
-      <c r="Q44" s="177"/>
-      <c r="R44" s="176"/>
-      <c r="S44" s="182" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E45" s="44" t="s">
-        <v>64</v>
+      <c r="H44" s="180"/>
+      <c r="I44" s="197" t="n">
+        <v>0.99806</v>
+      </c>
+      <c r="J44" s="231" t="n">
+        <v>1.8776</v>
+      </c>
+      <c r="K44" s="197" t="n">
+        <v>2.3451</v>
+      </c>
+      <c r="L44" s="250" t="n">
+        <v>1.3608</v>
+      </c>
+      <c r="M44" s="199" t="n">
+        <f aca="false">J44/((K44-L44)/I44)</f>
+        <v>1.90384786752007</v>
+      </c>
+      <c r="N44" s="65" t="n">
+        <f aca="false">((K44-J44)/(K44-L44))*100</f>
+        <v>47.4956822107081</v>
+      </c>
+      <c r="O44" s="72" t="n">
+        <f aca="false">P44-N44</f>
+        <v>4.75292908801109</v>
+      </c>
+      <c r="P44" s="67" t="n">
+        <f aca="false">(((K44-L44)-(J44/Q44)*I44)/(K44-L44))*100</f>
+        <v>52.2486112987192</v>
+      </c>
+      <c r="Q44" s="200" t="n">
+        <v>3.987</v>
+      </c>
+      <c r="R44" s="201" t="n">
+        <f aca="false">((J44*I44)/(Q44*(K44-L44)))*100</f>
+        <v>47.7513887012808</v>
+      </c>
+      <c r="S44" s="182" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E45" s="71" t="s">
+        <v>63</v>
       </c>
       <c r="F45" s="153"/>
       <c r="G45" s="153"/>
-      <c r="H45" s="178" t="n">
-        <v>70</v>
-      </c>
-      <c r="I45" s="156" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="J45" s="157" t="n">
-        <v>1.6498</v>
-      </c>
-      <c r="K45" s="157" t="n">
-        <v>2.2466</v>
-      </c>
-      <c r="L45" s="157" t="n">
-        <v>1.182</v>
-      </c>
-      <c r="M45" s="158" t="n">
+      <c r="H45" s="180"/>
+      <c r="I45" s="251" t="n">
+        <v>0.99806</v>
+      </c>
+      <c r="J45" s="197" t="n">
+        <v>1.9265</v>
+      </c>
+      <c r="K45" s="197" t="n">
+        <v>2.3725</v>
+      </c>
+      <c r="L45" s="197" t="n">
+        <v>1.3922</v>
+      </c>
+      <c r="M45" s="199" t="n">
         <f aca="false">J45/((K45-L45)/I45)</f>
-        <v>1.54662163817396</v>
-      </c>
-      <c r="N45" s="119" t="n">
+        <v>1.96140221360808</v>
+      </c>
+      <c r="N45" s="65" t="n">
         <f aca="false">((K45-J45)/(K45-L45))*100</f>
-        <v>56.0586135637798</v>
-      </c>
-      <c r="O45" s="159" t="n">
+        <v>45.4962766500051</v>
+      </c>
+      <c r="O45" s="72" t="n">
         <f aca="false">P45-N45</f>
-        <v>5.1497727373498</v>
-      </c>
-      <c r="P45" s="160" t="n">
+        <v>5.30878445839522</v>
+      </c>
+      <c r="P45" s="67" t="n">
         <f aca="false">(((K45-L45)-(J45/Q45)*I45)/(K45-L45))*100</f>
-        <v>61.2083863011296</v>
-      </c>
-      <c r="Q45" s="161" t="n">
+        <v>50.8050611084003</v>
+      </c>
+      <c r="Q45" s="200" t="n">
         <v>3.987</v>
       </c>
-      <c r="R45" s="160" t="n">
+      <c r="R45" s="201" t="n">
         <f aca="false">((J45*I45)/(Q45*(K45-L45)))*100</f>
-        <v>38.7916136988704</v>
-      </c>
-      <c r="S45" s="182" t="b">
+        <v>49.1949388915997</v>
+      </c>
+      <c r="S45" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E46" s="44"/>
+      <c r="E46" s="71"/>
       <c r="F46" s="153"/>
       <c r="G46" s="153"/>
-      <c r="H46" s="178"/>
-      <c r="I46" s="156" t="n">
-        <v>0.99802</v>
-      </c>
-      <c r="J46" s="157" t="n">
-        <v>1.4072</v>
-      </c>
-      <c r="K46" s="157" t="n">
-        <v>1.9133</v>
-      </c>
-      <c r="L46" s="157" t="n">
-        <v>1.0109</v>
-      </c>
-      <c r="M46" s="158" t="n">
+      <c r="H46" s="180"/>
+      <c r="I46" s="251" t="n">
+        <v>0.99806</v>
+      </c>
+      <c r="J46" s="197" t="n">
+        <v>1.9017</v>
+      </c>
+      <c r="K46" s="197" t="n">
+        <v>2.3704</v>
+      </c>
+      <c r="L46" s="197" t="n">
+        <v>1.3883</v>
+      </c>
+      <c r="M46" s="199" t="n">
         <f aca="false">J46/((K46-L46)/I46)</f>
-        <v>1.55630955673759</v>
-      </c>
-      <c r="N46" s="119" t="n">
+        <v>1.93260431931575</v>
+      </c>
+      <c r="N46" s="65" t="n">
         <f aca="false">((K46-J46)/(K46-L46))*100</f>
-        <v>56.0837765957447</v>
-      </c>
-      <c r="O46" s="159" t="n">
+        <v>47.7242643315345</v>
+      </c>
+      <c r="O46" s="72" t="n">
         <f aca="false">P46-N46</f>
-        <v>4.88162203135369</v>
-      </c>
-      <c r="P46" s="160" t="n">
+        <v>3.80309159232426</v>
+      </c>
+      <c r="P46" s="67" t="n">
         <f aca="false">(((K46-L46)-(J46/Q46)*I46)/(K46-L46))*100</f>
-        <v>60.9653986270984</v>
-      </c>
-      <c r="Q46" s="161" t="n">
+        <v>51.5273559238588</v>
+      </c>
+      <c r="Q46" s="200" t="n">
         <v>3.987</v>
       </c>
-      <c r="R46" s="160" t="n">
+      <c r="R46" s="201" t="n">
         <f aca="false">((J46*I46)/(Q46*(K46-L46)))*100</f>
-        <v>39.0346013729016</v>
-      </c>
-      <c r="S46" s="182" t="b">
+        <v>48.4726440761413</v>
+      </c>
+      <c r="S46" s="182" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E47" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="F47" s="153"/>
-      <c r="G47" s="153"/>
-      <c r="H47" s="180" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I47" s="60" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="J47" s="71" t="n">
-        <v>1.8318</v>
-      </c>
-      <c r="K47" s="60" t="n">
-        <v>2.3194</v>
-      </c>
-      <c r="L47" s="60" t="n">
-        <v>1.3364</v>
-      </c>
-      <c r="M47" s="64" t="n">
-        <f aca="false">J47/((K47-L47)/I47)</f>
-        <v>1.85986399593082</v>
-      </c>
-      <c r="N47" s="65" t="n">
-        <f aca="false">((K47-J47)/(K47-L47))*100</f>
-        <v>49.6032553407935</v>
-      </c>
-      <c r="O47" s="66" t="n">
-        <f aca="false">P47-N47</f>
-        <v>3.74853808958464</v>
-      </c>
-      <c r="P47" s="67" t="n">
-        <f aca="false">(((K47-L47)-(J47/Q47)*I47)/(K47-L47))*100</f>
-        <v>53.3517934303781</v>
-      </c>
-      <c r="Q47" s="68" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R47" s="69" t="n">
-        <f aca="false">((J47*I47)/(Q47*(K47-L47)))*100</f>
-        <v>46.6482065696219</v>
-      </c>
-      <c r="S47" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="60"/>
-      <c r="F48" s="153"/>
-      <c r="G48" s="153"/>
-      <c r="H48" s="180"/>
-      <c r="I48" s="60" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="J48" s="71" t="n">
-        <v>1.8776</v>
-      </c>
-      <c r="K48" s="60" t="n">
-        <v>2.3451</v>
-      </c>
-      <c r="L48" s="171" t="n">
-        <v>1.3608</v>
-      </c>
-      <c r="M48" s="64" t="n">
-        <f aca="false">J48/((K48-L48)/I48)</f>
-        <v>1.90384786752007</v>
-      </c>
-      <c r="N48" s="65" t="n">
-        <f aca="false">((K48-J48)/(K48-L48))*100</f>
-        <v>47.4956822107081</v>
-      </c>
-      <c r="O48" s="72" t="n">
-        <f aca="false">P48-N48</f>
-        <v>4.75292908801109</v>
-      </c>
-      <c r="P48" s="67" t="n">
-        <f aca="false">(((K48-L48)-(J48/Q48)*I48)/(K48-L48))*100</f>
-        <v>52.2486112987192</v>
-      </c>
-      <c r="Q48" s="73" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R48" s="67" t="n">
-        <f aca="false">((J48*I48)/(Q48*(K48-L48)))*100</f>
-        <v>47.7513887012808</v>
-      </c>
-      <c r="S48" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E49" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="F49" s="153"/>
-      <c r="G49" s="153"/>
-      <c r="H49" s="180"/>
-      <c r="I49" s="181" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="J49" s="60" t="n">
-        <v>1.9265</v>
-      </c>
-      <c r="K49" s="60" t="n">
-        <v>2.3725</v>
-      </c>
-      <c r="L49" s="60" t="n">
-        <v>1.3922</v>
-      </c>
-      <c r="M49" s="64" t="n">
-        <f aca="false">J49/((K49-L49)/I49)</f>
-        <v>1.96140221360808</v>
-      </c>
-      <c r="N49" s="65" t="n">
-        <f aca="false">((K49-J49)/(K49-L49))*100</f>
-        <v>45.4962766500051</v>
-      </c>
-      <c r="O49" s="72" t="n">
-        <f aca="false">P49-N49</f>
-        <v>5.30878445839522</v>
-      </c>
-      <c r="P49" s="67" t="n">
-        <f aca="false">(((K49-L49)-(J49/Q49)*I49)/(K49-L49))*100</f>
-        <v>50.8050611084003</v>
-      </c>
-      <c r="Q49" s="73" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R49" s="67" t="n">
-        <f aca="false">((J49*I49)/(Q49*(K49-L49)))*100</f>
-        <v>49.1949388915997</v>
-      </c>
-      <c r="S49" s="182" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="71"/>
-      <c r="F50" s="153"/>
-      <c r="G50" s="153"/>
-      <c r="H50" s="180"/>
-      <c r="I50" s="181" t="n">
-        <v>0.99806</v>
-      </c>
-      <c r="J50" s="60" t="n">
-        <v>1.9017</v>
-      </c>
-      <c r="K50" s="60" t="n">
-        <v>2.3704</v>
-      </c>
-      <c r="L50" s="60" t="n">
-        <v>1.3883</v>
-      </c>
-      <c r="M50" s="64" t="n">
-        <f aca="false">J50/((K50-L50)/I50)</f>
-        <v>1.93260431931575</v>
-      </c>
-      <c r="N50" s="65" t="n">
-        <f aca="false">((K50-J50)/(K50-L50))*100</f>
-        <v>47.7242643315345</v>
-      </c>
-      <c r="O50" s="72" t="n">
-        <f aca="false">P50-N50</f>
-        <v>3.80309159232426</v>
-      </c>
-      <c r="P50" s="67" t="n">
-        <f aca="false">(((K50-L50)-(J50/Q50)*I50)/(K50-L50))*100</f>
-        <v>51.5273559238588</v>
-      </c>
-      <c r="Q50" s="73" t="n">
-        <v>3.987</v>
-      </c>
-      <c r="R50" s="67" t="n">
-        <f aca="false">((J50*I50)/(Q50*(K50-L50)))*100</f>
-        <v>48.4726440761413</v>
-      </c>
-      <c r="S50" s="182" t="b">
-        <v>0</v>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H56" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="H43:H46"/>
     <mergeCell ref="E45:E46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="E49:E50"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8640,13 +8250,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.85"/>
@@ -8659,110 +8269,63 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="183" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="H2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>31</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>33.33</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>35.4</v>
-      </c>
-      <c r="G3" s="4" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>31</v>
-      </c>
-      <c r="I3" s="4" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="85" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>69</v>
-      </c>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="252"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="252"/>
+      <c r="B2" s="252"/>
+      <c r="C2" s="252"/>
+      <c r="D2" s="252"/>
+      <c r="E2" s="252"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="85"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A5" s="97"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="183" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="183"/>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
+      <c r="A7" s="252" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="252"/>
+      <c r="C7" s="252"/>
+      <c r="D7" s="252"/>
+      <c r="E7" s="252"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="183"/>
-      <c r="B8" s="183"/>
-      <c r="C8" s="183"/>
-      <c r="D8" s="183"/>
-      <c r="E8" s="183"/>
+      <c r="A8" s="252"/>
+      <c r="B8" s="252"/>
+      <c r="C8" s="252"/>
+      <c r="D8" s="252"/>
+      <c r="E8" s="252"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="n">
@@ -8789,33 +8352,36 @@
       <c r="I9" s="4" t="n">
         <v>70</v>
       </c>
+      <c r="J9" s="253" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="184" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="184" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="184" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="187" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="188" t="s">
+      <c r="B10" s="254" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="254" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="254" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="257" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="258" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8823,145 +8389,145 @@
       <c r="A11" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="184" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="186" t="s">
-        <v>71</v>
+      <c r="B11" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="254" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="256" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="184" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="186" t="s">
-        <v>71</v>
+        <v>78</v>
+      </c>
+      <c r="B12" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="254" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="256" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="184" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="186" t="s">
-        <v>71</v>
+        <v>79</v>
+      </c>
+      <c r="B13" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="254" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="256" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="171" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="189" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="187" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="188" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="259" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="257" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="258" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="186" t="s">
-        <v>71</v>
+      <c r="I14" s="256" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="185" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="189" t="s">
-        <v>76</v>
-      </c>
-      <c r="H15" s="186" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="189" t="s">
-        <v>76</v>
+      <c r="B15" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="259" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="256" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="259" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -8990,153 +8556,153 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="104"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="190" t="s">
-        <v>77</v>
+      <c r="A1" s="260" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="190"/>
+      <c r="A2" s="260"/>
     </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="191" t="s">
-        <v>78</v>
+      <c r="A3" s="261" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="191" t="s">
-        <v>79</v>
+      <c r="A4" s="261" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="191" t="s">
-        <v>80</v>
+      <c r="A5" s="261" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="191"/>
+      <c r="A6" s="261"/>
     </row>
     <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="191"/>
+      <c r="A7" s="261"/>
     </row>
     <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="191"/>
+      <c r="A8" s="261"/>
     </row>
     <row r="9" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="191"/>
+      <c r="A9" s="261"/>
     </row>
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="191"/>
+      <c r="A10" s="261"/>
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="191"/>
+      <c r="A11" s="261"/>
     </row>
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="191"/>
+      <c r="A12" s="261"/>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="191"/>
+      <c r="A13" s="261"/>
     </row>
     <row r="14" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="191"/>
+      <c r="A14" s="261"/>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="191"/>
+      <c r="A15" s="261"/>
     </row>
     <row r="16" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="191"/>
+      <c r="A16" s="261"/>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="191"/>
+      <c r="A17" s="261"/>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="191"/>
+      <c r="A18" s="261"/>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="191"/>
+      <c r="A19" s="261"/>
     </row>
     <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="191"/>
+      <c r="A20" s="261"/>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="191"/>
+      <c r="A21" s="261"/>
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="191"/>
+      <c r="A22" s="261"/>
     </row>
     <row r="23" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="191"/>
+      <c r="A23" s="261"/>
     </row>
     <row r="24" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="191"/>
+      <c r="A24" s="261"/>
     </row>
     <row r="25" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="191"/>
+      <c r="A25" s="261"/>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="191"/>
+      <c r="A26" s="261"/>
     </row>
     <row r="27" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="191"/>
+      <c r="A27" s="261"/>
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="191"/>
+      <c r="A28" s="261"/>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="191"/>
+      <c r="A29" s="261"/>
     </row>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="191"/>
+      <c r="A30" s="261"/>
     </row>
     <row r="31" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="191"/>
+      <c r="A31" s="261"/>
     </row>
     <row r="32" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="191"/>
+      <c r="A32" s="261"/>
     </row>
     <row r="33" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="191"/>
+      <c r="A33" s="261"/>
     </row>
     <row r="34" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="191"/>
+      <c r="A34" s="261"/>
     </row>
     <row r="35" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="191"/>
+      <c r="A35" s="261"/>
     </row>
     <row r="36" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="191"/>
+      <c r="A36" s="261"/>
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="191"/>
+      <c r="A37" s="261"/>
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="191"/>
+      <c r="A38" s="261"/>
     </row>
     <row r="39" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="191"/>
+      <c r="A39" s="261"/>
     </row>
     <row r="40" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="191"/>
+      <c r="A40" s="261"/>
     </row>
     <row r="41" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="191"/>
+      <c r="A41" s="261"/>
     </row>
     <row r="42" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="191"/>
+      <c r="A42" s="261"/>
     </row>
     <row r="43" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="191"/>
+      <c r="A43" s="261"/>
     </row>
     <row r="44" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="191"/>
+      <c r="A44" s="261"/>
     </row>
     <row r="45" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="191"/>
+      <c r="A45" s="261"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>